<commit_message>
Added location and taxa information to Example dataset
</commit_message>
<xml_diff>
--- a/docs/data_providers/data_format/Example.xlsx
+++ b/docs/data_providers/data_format/Example.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/docs/data_providers/data_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147944BF-0842-904F-A890-D4C92E4AB976}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82351ABE-5928-5048-A3B2-B1E737CA7E4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7780" yWindow="500" windowWidth="27360" windowHeight="16940" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="27360" windowHeight="16940" activeTab="3" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="GBIFTaxa" sheetId="2" r:id="rId2"/>
+    <sheet name="NCBITaxa" sheetId="3" r:id="rId3"/>
+    <sheet name="Locations" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="122">
   <si>
     <t>Title</t>
   </si>
@@ -178,6 +181,219 @@
   </si>
   <si>
     <t>GeoJSON file containing polylines of the bait trap transects</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Taxon name</t>
+  </si>
+  <si>
+    <t>Taxon type</t>
+  </si>
+  <si>
+    <t>Taxon ID</t>
+  </si>
+  <si>
+    <t>Ignore ID</t>
+  </si>
+  <si>
+    <t>Parent type</t>
+  </si>
+  <si>
+    <t>Parent name</t>
+  </si>
+  <si>
+    <t>Parent ID</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>crbo</t>
+  </si>
+  <si>
+    <t>Crematogaster borneensis</t>
+  </si>
+  <si>
+    <t>Species</t>
+  </si>
+  <si>
+    <t>dolic_sp</t>
+  </si>
+  <si>
+    <t>Dolichoderus</t>
+  </si>
+  <si>
+    <t>Genus</t>
+  </si>
+  <si>
+    <t>gannets</t>
+  </si>
+  <si>
+    <t>Morus</t>
+  </si>
+  <si>
+    <t>lost_orang</t>
+  </si>
+  <si>
+    <t>Pongo tapanuliensis</t>
+  </si>
+  <si>
+    <t>Pongo</t>
+  </si>
+  <si>
+    <t>New species</t>
+  </si>
+  <si>
+    <t>morpho1</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Morphospecies</t>
+  </si>
+  <si>
+    <t>Formicidae</t>
+  </si>
+  <si>
+    <t>Family</t>
+  </si>
+  <si>
+    <t>bombines</t>
+  </si>
+  <si>
+    <t>Bombini</t>
+  </si>
+  <si>
+    <t>Tribe</t>
+  </si>
+  <si>
+    <t>Apidae</t>
+  </si>
+  <si>
+    <t>micr_hid</t>
+  </si>
+  <si>
+    <t>Microcopris hidakai</t>
+  </si>
+  <si>
+    <t>Microcopris</t>
+  </si>
+  <si>
+    <t>New</t>
+  </si>
+  <si>
+    <t>Superkingdom</t>
+  </si>
+  <si>
+    <t>Kingdom</t>
+  </si>
+  <si>
+    <t>Phylum</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>G_proteobacteria</t>
+  </si>
+  <si>
+    <t>Bacteria</t>
+  </si>
+  <si>
+    <t>Pseudomonadota</t>
+  </si>
+  <si>
+    <t>Gammaproteobacteria</t>
+  </si>
+  <si>
+    <t>E_mycetes</t>
+  </si>
+  <si>
+    <t>Eukaryota</t>
+  </si>
+  <si>
+    <t>Fungi</t>
+  </si>
+  <si>
+    <t>Ascomycota</t>
+  </si>
+  <si>
+    <t>Eurotiomycetes</t>
+  </si>
+  <si>
+    <t>Dinophyceae</t>
+  </si>
+  <si>
+    <t>Acidobact</t>
+  </si>
+  <si>
+    <t>k__Bacteria</t>
+  </si>
+  <si>
+    <t>p__Acidobacteria</t>
+  </si>
+  <si>
+    <t>c__Acidobacteriia</t>
+  </si>
+  <si>
+    <t>New_fungus</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Mynewfungusetes</t>
+  </si>
+  <si>
+    <t>Location name</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>WKT</t>
+  </si>
+  <si>
+    <t>E_194</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>E_195</t>
+  </si>
+  <si>
+    <t>My_site_1</t>
+  </si>
+  <si>
+    <t>POINT</t>
+  </si>
+  <si>
+    <t>My_site_2</t>
+  </si>
+  <si>
+    <t>My_site_3</t>
+  </si>
+  <si>
+    <t>Point(117.7762 4.9576)</t>
+  </si>
+  <si>
+    <t>My_transect_1</t>
+  </si>
+  <si>
+    <t>Linestring</t>
+  </si>
+  <si>
+    <t>Linestring(117.7762 4.9576, 117.7862 4.9676)</t>
   </si>
 </sst>
 </file>
@@ -222,10 +438,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -543,14 +760,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56835824-9479-A543-9F3B-4D7006FD1F4E}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -799,4 +1016,477 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AE1033-5819-974F-8B61-434FB3A99D80}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2480962</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3">
+        <v>1090433</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95D2376D-CAF7-794F-A21C-41734DBF2E1E}">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B70BB96-69CE-5C4B-B649-6188C128ED73}">
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="3">
+        <v>4.9577210000000003</v>
+      </c>
+      <c r="D4" s="3">
+        <v>117.776023</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added example datasheets to the example file
</commit_message>
<xml_diff>
--- a/docs/data_providers/data_format/Example.xlsx
+++ b/docs/data_providers/data_format/Example.xlsx
@@ -8,15 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/docs/data_providers/data_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82351ABE-5928-5048-A3B2-B1E737CA7E4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE42B77-E40E-E34E-88D6-713459C4567D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="27360" windowHeight="16940" activeTab="3" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="27360" windowHeight="16940" activeTab="10" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="GBIFTaxa" sheetId="2" r:id="rId2"/>
     <sheet name="NCBITaxa" sheetId="3" r:id="rId3"/>
     <sheet name="Locations" sheetId="4" r:id="rId4"/>
+    <sheet name="abundances_1" sheetId="5" r:id="rId5"/>
+    <sheet name="abundances_2" sheetId="6" r:id="rId6"/>
+    <sheet name="interactions_1" sheetId="7" r:id="rId7"/>
+    <sheet name="interactions_2" sheetId="8" r:id="rId8"/>
+    <sheet name="interactions_3" sheetId="9" r:id="rId9"/>
+    <sheet name="external_1" sheetId="10" r:id="rId10"/>
+    <sheet name="external_2" sheetId="11" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="187">
   <si>
     <t>Title</t>
   </si>
@@ -394,13 +401,208 @@
   </si>
   <si>
     <t>Linestring(117.7762 4.9576, 117.7862 4.9676)</t>
+  </si>
+  <si>
+    <t>field_type</t>
+  </si>
+  <si>
+    <t>Abundance</t>
+  </si>
+  <si>
+    <t>taxon_name</t>
+  </si>
+  <si>
+    <t>Tiger leech</t>
+  </si>
+  <si>
+    <t>Brown leech</t>
+  </si>
+  <si>
+    <t>method</t>
+  </si>
+  <si>
+    <t>Exhaustive search of 50cm quadrat</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>quadrat count</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>individuals</t>
+  </si>
+  <si>
+    <t>field_name</t>
+  </si>
+  <si>
+    <t>tiger_count</t>
+  </si>
+  <si>
+    <t>brown_count</t>
+  </si>
+  <si>
+    <t>Taxa</t>
+  </si>
+  <si>
+    <t>taxon_field</t>
+  </si>
+  <si>
+    <t>common_name</t>
+  </si>
+  <si>
+    <t>Species found</t>
+  </si>
+  <si>
+    <t>Number found</t>
+  </si>
+  <si>
+    <t>leech_count</t>
+  </si>
+  <si>
+    <t>Taxon</t>
+  </si>
+  <si>
+    <t>Categorical Interaction</t>
+  </si>
+  <si>
+    <t>interaction_field</t>
+  </si>
+  <si>
+    <t>predator;prey</t>
+  </si>
+  <si>
+    <t>levels</t>
+  </si>
+  <si>
+    <t>success;failure</t>
+  </si>
+  <si>
+    <t>Visual observation</t>
+  </si>
+  <si>
+    <t>Predator observed</t>
+  </si>
+  <si>
+    <t>Prey observed</t>
+  </si>
+  <si>
+    <t>Outcome of predation event</t>
+  </si>
+  <si>
+    <t>predator</t>
+  </si>
+  <si>
+    <t>prey</t>
+  </si>
+  <si>
+    <t>outcome</t>
+  </si>
+  <si>
+    <t>Clouded leopard</t>
+  </si>
+  <si>
+    <t>Brown rat</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>Flat headed cat</t>
+  </si>
+  <si>
+    <t>Moon rat</t>
+  </si>
+  <si>
+    <t>failure</t>
+  </si>
+  <si>
+    <t>interaction_name</t>
+  </si>
+  <si>
+    <t>Clouded leopard:predator;Brown rat:prey</t>
+  </si>
+  <si>
+    <t>Clouded leopard:predator;</t>
+  </si>
+  <si>
+    <t>prey:prey species;</t>
+  </si>
+  <si>
+    <t>Numeric</t>
+  </si>
+  <si>
+    <t>File</t>
+  </si>
+  <si>
+    <t>Altitude in metres</t>
+  </si>
+  <si>
+    <t>DEM file used for altitude</t>
+  </si>
+  <si>
+    <t>Extracted from DEM tiffs</t>
+  </si>
+  <si>
+    <t>metres</t>
+  </si>
+  <si>
+    <t>Altitude</t>
+  </si>
+  <si>
+    <t>DEM</t>
+  </si>
+  <si>
+    <t>My_raster_1.tiff</t>
+  </si>
+  <si>
+    <t>My_raster_2.tiff</t>
+  </si>
+  <si>
+    <t>Image of Quadrat</t>
+  </si>
+  <si>
+    <t>file_container</t>
+  </si>
+  <si>
+    <t>My_archive.zip</t>
+  </si>
+  <si>
+    <t>Quadrat_image</t>
+  </si>
+  <si>
+    <t>Site_quadrat_1.jpg</t>
+  </si>
+  <si>
+    <t>Site_quadrat_2.jpg</t>
+  </si>
+  <si>
+    <t>Site_quadrat_3.jpg</t>
+  </si>
+  <si>
+    <t>Site_quadrat_4.jpg</t>
+  </si>
+  <si>
+    <t>Site_quadrat_5.jpg</t>
+  </si>
+  <si>
+    <t>Site_quadrat_6.jpg</t>
+  </si>
+  <si>
+    <t>Site_quadrat_7.jpg</t>
+  </si>
+  <si>
+    <t>Site_quadrat_8.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -412,6 +614,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,11 +648,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1018,6 +1229,346 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4564A69-1797-E343-B331-4E4216D5E9E0}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>100</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3">
+        <v>200</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>300</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3">
+        <v>400</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>5</v>
+      </c>
+      <c r="B11" s="3">
+        <v>500</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3">
+        <v>600</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3">
+        <v>700</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>8</v>
+      </c>
+      <c r="B14" s="3">
+        <v>800</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA611AD8-B75D-FF4F-B5EC-A2F06456CF6C}">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3">
+        <v>100</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3">
+        <v>200</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>3</v>
+      </c>
+      <c r="B10" s="3">
+        <v>300</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3">
+        <v>400</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>5</v>
+      </c>
+      <c r="B12" s="3">
+        <v>500</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
+        <v>600</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3">
+        <v>700</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3">
+        <v>800</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AE1033-5819-974F-8B61-434FB3A99D80}">
   <dimension ref="A1:I8"/>
@@ -1348,7 +1899,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B70BB96-69CE-5C4B-B649-6188C128ED73}">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
@@ -1489,4 +2040,592 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB2131-D12F-E446-A544-0D39287054FC}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="30.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3">
+        <v>24</v>
+      </c>
+      <c r="C7" s="3">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3">
+        <v>62</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C9608A4-A834-0C4F-97DF-49D93E72537D}">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C7" s="3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C8" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="3">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB73AB8-5ABC-CC46-A983-918430EF84FB}">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7854E2C-1FBE-7947-BDF9-5436657A8287}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>2</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68319B6E-55A5-CD40-8D21-94807C1DFFAF}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>2</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added steps to display summary data from example file
</commit_message>
<xml_diff>
--- a/docs/data_providers/data_format/Example.xlsx
+++ b/docs/data_providers/data_format/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/docs/data_providers/data_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE42B77-E40E-E34E-88D6-713459C4567D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54C4B89-238E-5643-AC2C-224803E7AF12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="27360" windowHeight="16940" activeTab="10" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="27360" windowHeight="16940" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="188">
   <si>
     <t>Title</t>
   </si>
@@ -596,6 +596,9 @@
   </si>
   <si>
     <t>Site_quadrat_8.jpg</t>
+  </si>
+  <si>
+    <t>Worksheet description</t>
   </si>
 </sst>
 </file>
@@ -969,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56835824-9479-A543-9F3B-4D7006FD1F4E}">
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1071,159 +1074,164 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>22</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>24</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>25</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
         <v>33</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>34</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>35</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B26" s="1">
         <v>42156</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B27" s="1">
         <v>42196</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>41</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>5.07</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>42</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>4.5</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>43</v>
       </c>
-      <c r="B29">
+      <c r="B30">
         <v>117.82</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
         <v>44</v>
       </c>
-      <c r="B30">
+      <c r="B31">
         <v>116.75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B8" r:id="rId1" xr:uid="{8F2F57F5-1AEE-0D48-93D7-9691DA786243}"/>
-    <hyperlink ref="B17" r:id="rId2" xr:uid="{854E441D-2155-F243-9B6D-EA2BAFB9B5A2}"/>
-    <hyperlink ref="B21" r:id="rId3" xr:uid="{1F970723-7B44-4944-98C3-9AB1AB233E97}"/>
+    <hyperlink ref="B18" r:id="rId2" xr:uid="{854E441D-2155-F243-9B6D-EA2BAFB9B5A2}"/>
+    <hyperlink ref="B22" r:id="rId3" xr:uid="{1F970723-7B44-4944-98C3-9AB1AB233E97}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1398,7 +1406,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA611AD8-B75D-FF4F-B5EC-A2F06456CF6C}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated Example dataset so that it should pass validation
</commit_message>
<xml_diff>
--- a/docs/data_providers/data_format/Example.xlsx
+++ b/docs/data_providers/data_format/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/docs/data_providers/data_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D54C4B89-238E-5643-AC2C-224803E7AF12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5599A200-C61E-6341-B716-4881F6352AD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="27360" windowHeight="16940" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="27360" windowHeight="16940" activeTab="1" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -103,9 +103,6 @@
     <t>External file</t>
   </si>
   <si>
-    <t>External file descripton</t>
-  </si>
-  <si>
     <t>Publication DOI</t>
   </si>
   <si>
@@ -599,6 +596,9 @@
   </si>
   <si>
     <t>Worksheet description</t>
+  </si>
+  <si>
+    <t>External file description</t>
   </si>
 </sst>
 </file>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56835824-9479-A543-9F3B-4D7006FD1F4E}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1022,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="1">
-        <v>43711</v>
+        <v>46156</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1074,7 +1074,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1087,10 +1087,10 @@
         <v>20</v>
       </c>
       <c r="B15" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1098,90 +1098,90 @@
         <v>21</v>
       </c>
       <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
         <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>187</v>
       </c>
       <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
         <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1">
         <v>42156</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27" s="1">
         <v>42196</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>5.07</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B29">
         <v>4.5</v>
@@ -1213,7 +1213,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B30">
         <v>117.82</v>
@@ -1221,7 +1221,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B31">
         <v>116.75</v>
@@ -1253,60 +1253,60 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
         <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1328,7 +1328,7 @@
         <v>200</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1339,7 +1339,7 @@
         <v>300</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>400</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
         <v>500</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1372,7 +1372,7 @@
         <v>600</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1383,7 +1383,7 @@
         <v>700</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1394,7 +1394,7 @@
         <v>800</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -1419,69 +1419,69 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1492,7 +1492,7 @@
         <v>100</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1503,7 +1503,7 @@
         <v>200</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1514,7 +1514,7 @@
         <v>300</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1525,7 +1525,7 @@
         <v>400</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1536,7 +1536,7 @@
         <v>500</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1547,7 +1547,7 @@
         <v>600</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1558,7 +1558,7 @@
         <v>700</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1569,7 +1569,7 @@
         <v>800</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
@@ -1581,8 +1581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AE1033-5819-974F-8B61-434FB3A99D80}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1596,42 +1596,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -1642,13 +1642,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1659,13 +1659,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>67</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" s="3">
         <v>2480962</v>
@@ -1678,88 +1678,88 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>79</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>82</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3">
         <v>1090433</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
@@ -1788,113 +1788,113 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>102</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>105</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -1923,30 +1923,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1955,10 +1955,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1967,10 +1967,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C4" s="3">
         <v>4.9577210000000003</v>
@@ -1979,70 +1979,70 @@
         <v>117.776023</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>117</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2065,73 +2065,73 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>123</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>126</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="C3" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>130</v>
-      </c>
       <c r="C4" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>132</v>
-      </c>
       <c r="C5" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>134</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>135</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -2211,62 +2211,62 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>139</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2274,7 +2274,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="3">
         <v>24</v>
@@ -2285,7 +2285,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="3">
         <v>12</v>
@@ -2296,7 +2296,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C9" s="3">
         <v>62</v>
@@ -2307,7 +2307,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" s="3">
         <v>3</v>
@@ -2335,78 +2335,78 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2414,13 +2414,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2428,13 +2428,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -2458,50 +2458,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2509,7 +2509,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2517,7 +2517,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>
@@ -2542,73 +2542,73 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>142</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2616,10 +2616,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2627,10 +2627,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated taxonomy to so that GBIF part of example file passes validation
</commit_message>
<xml_diff>
--- a/docs/data_providers/data_format/Example.xlsx
+++ b/docs/data_providers/data_format/Example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/docs/data_providers/data_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5599A200-C61E-6341-B716-4881F6352AD4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C7EE9D-9498-7342-A3A2-F5B2F926A6DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="27360" windowHeight="16940" activeTab="1" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="188">
   <si>
     <t>Title</t>
   </si>
@@ -277,15 +277,6 @@
     <t>Apidae</t>
   </si>
   <si>
-    <t>micr_hid</t>
-  </si>
-  <si>
-    <t>Microcopris hidakai</t>
-  </si>
-  <si>
-    <t>Microcopris</t>
-  </si>
-  <si>
     <t>New</t>
   </si>
   <si>
@@ -599,6 +590,15 @@
   </si>
   <si>
     <t>External file description</t>
+  </si>
+  <si>
+    <t>Morus rubra</t>
+  </si>
+  <si>
+    <t>new_gannet</t>
+  </si>
+  <si>
+    <t>New gannet (not mulberry) species</t>
   </si>
 </sst>
 </file>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1106,7 +1106,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B17" t="s">
         <v>48</v>
@@ -1253,60 +1253,60 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1317,7 +1317,7 @@
         <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1328,7 +1328,7 @@
         <v>200</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1339,7 +1339,7 @@
         <v>300</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,7 +1350,7 @@
         <v>400</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1361,7 +1361,7 @@
         <v>500</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1372,7 +1372,7 @@
         <v>600</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1383,7 +1383,7 @@
         <v>700</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1394,7 +1394,7 @@
         <v>800</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1419,69 +1419,69 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1492,7 +1492,7 @@
         <v>100</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1503,7 +1503,7 @@
         <v>200</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1514,7 +1514,7 @@
         <v>300</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1525,7 +1525,7 @@
         <v>400</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1536,7 +1536,7 @@
         <v>500</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1547,7 +1547,7 @@
         <v>600</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1558,7 +1558,7 @@
         <v>700</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1569,7 +1569,7 @@
         <v>800</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1582,7 +1582,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1592,6 +1592,7 @@
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -1743,26 +1744,30 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>80</v>
+        <v>186</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="E8" s="3">
-        <v>1090433</v>
+      <c r="E8">
+        <v>5361886</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="H8" s="3">
+        <v>2480962</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>187</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1791,19 +1796,19 @@
         <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>87</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>58</v>
@@ -1811,90 +1816,90 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -1923,30 +1928,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1955,10 +1960,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1967,10 +1972,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C4" s="3">
         <v>4.9577210000000003</v>
@@ -1979,7 +1984,7 @@
         <v>117.776023</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>72</v>
@@ -1987,10 +1992,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>72</v>
@@ -1999,7 +2004,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>72</v>
@@ -2007,10 +2012,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>72</v>
@@ -2019,18 +2024,18 @@
         <v>72</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>72</v>
@@ -2039,10 +2044,10 @@
         <v>72</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2065,73 +2070,73 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -2211,62 +2216,62 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2274,7 +2279,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C7" s="3">
         <v>24</v>
@@ -2285,7 +2290,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C8" s="3">
         <v>12</v>
@@ -2296,7 +2301,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C9" s="3">
         <v>62</v>
@@ -2307,7 +2312,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C10" s="3">
         <v>3</v>
@@ -2335,78 +2340,78 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2414,13 +2419,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2428,13 +2433,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2458,50 +2463,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2509,7 +2514,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2517,7 +2522,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -2542,73 +2547,73 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2616,10 +2621,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2627,10 +2632,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added worksheet details to example file and fixed all the validation errors that then arose
</commit_message>
<xml_diff>
--- a/docs/data_providers/data_format/Example.xlsx
+++ b/docs/data_providers/data_format/Example.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc2017/Documents/MyRepos/safedata_validator/docs/data_providers/data_format/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C7EE9D-9498-7342-A3A2-F5B2F926A6DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE3DD28-562F-EF46-BB9F-5B8DE1CA9D52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="27360" windowHeight="16940" activeTab="1" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="27360" windowHeight="16940" xr2:uid="{958BE4CB-34F0-9B46-9A32-339A0F6D953C}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="213">
   <si>
     <t>Title</t>
   </si>
@@ -178,15 +178,9 @@
     <t>bait_trap_images.zip</t>
   </si>
   <si>
-    <t>BaitTrapTransects.geojson</t>
-  </si>
-  <si>
     <t>Zip file containing 5000 JPEG images of bait trap cards</t>
   </si>
   <si>
-    <t>GeoJSON file containing polylines of the bait trap transects</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -451,9 +445,6 @@
     <t>leech_count</t>
   </si>
   <si>
-    <t>Taxon</t>
-  </si>
-  <si>
     <t>Categorical Interaction</t>
   </si>
   <si>
@@ -550,18 +541,9 @@
     <t>My_raster_2.tiff</t>
   </si>
   <si>
-    <t>Image of Quadrat</t>
-  </si>
-  <si>
     <t>file_container</t>
   </si>
   <si>
-    <t>My_archive.zip</t>
-  </si>
-  <si>
-    <t>Quadrat_image</t>
-  </si>
-  <si>
     <t>Site_quadrat_1.jpg</t>
   </si>
   <si>
@@ -599,6 +581,99 @@
   </si>
   <si>
     <t>New gannet (not mulberry) species</t>
+  </si>
+  <si>
+    <t>abundances_1</t>
+  </si>
+  <si>
+    <t>Abundances example 1</t>
+  </si>
+  <si>
+    <t>abundances_2</t>
+  </si>
+  <si>
+    <t>Abundances example 2</t>
+  </si>
+  <si>
+    <t>Example worksheet showing the second method for recording species abundances</t>
+  </si>
+  <si>
+    <t>Example worksheet showing the first method for recording species abundances</t>
+  </si>
+  <si>
+    <t>interactions_1</t>
+  </si>
+  <si>
+    <t>interactions_2</t>
+  </si>
+  <si>
+    <t>interactions_3</t>
+  </si>
+  <si>
+    <t>Interactions example 1</t>
+  </si>
+  <si>
+    <t>Interactions example 2</t>
+  </si>
+  <si>
+    <t>Interactions example 3</t>
+  </si>
+  <si>
+    <t>Example worksheet showing the first method for recording species interactions</t>
+  </si>
+  <si>
+    <t>Example worksheet showing the second method for recording species interactions</t>
+  </si>
+  <si>
+    <t>Example worksheet showing the third method for recording species interactions</t>
+  </si>
+  <si>
+    <t>external_1</t>
+  </si>
+  <si>
+    <t>external_2</t>
+  </si>
+  <si>
+    <t>External file example 1</t>
+  </si>
+  <si>
+    <t>External file example 2</t>
+  </si>
+  <si>
+    <t>Example worksheet showing the first method for including information from external files</t>
+  </si>
+  <si>
+    <t>Example worksheet showing the secod method for including information from external files</t>
+  </si>
+  <si>
+    <t>Haemadipsa picta</t>
+  </si>
+  <si>
+    <t>Haemadipsa zeylanica</t>
+  </si>
+  <si>
+    <t>Neofelis nebulosa</t>
+  </si>
+  <si>
+    <t>Prionailurus planiceps</t>
+  </si>
+  <si>
+    <t>Rattus norvegicus</t>
+  </si>
+  <si>
+    <t>Echinosorex gymnura</t>
+  </si>
+  <si>
+    <t>Image of bait trap card</t>
+  </si>
+  <si>
+    <t>Bait_trap_image</t>
+  </si>
+  <si>
+    <t>A raster file containing altitudes</t>
+  </si>
+  <si>
+    <t>A second raster file containing altitudes</t>
   </si>
 </sst>
 </file>
@@ -972,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56835824-9479-A543-9F3B-4D7006FD1F4E}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -983,9 +1058,11 @@
     <col min="1" max="1" width="20.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="42.5" customWidth="1"/>
     <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -993,7 +1070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1001,7 +1078,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1009,7 +1086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1017,7 +1094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1025,12 +1102,12 @@
         <v>46156</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1038,7 +1115,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1046,7 +1123,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1054,7 +1131,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -1062,27 +1139,90 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>182</v>
+      </c>
+      <c r="C11" t="s">
+        <v>184</v>
+      </c>
+      <c r="D11" t="s">
+        <v>188</v>
+      </c>
+      <c r="E11" t="s">
+        <v>189</v>
+      </c>
+      <c r="F11" t="s">
+        <v>190</v>
+      </c>
+      <c r="G11" t="s">
+        <v>197</v>
+      </c>
+      <c r="H11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>183</v>
+      </c>
+      <c r="C12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D12" t="s">
+        <v>191</v>
+      </c>
+      <c r="E12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G12" t="s">
+        <v>199</v>
+      </c>
+      <c r="H12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+      <c r="B13" t="s">
+        <v>187</v>
+      </c>
+      <c r="C13" t="s">
+        <v>186</v>
+      </c>
+      <c r="D13" t="s">
+        <v>194</v>
+      </c>
+      <c r="E13" t="s">
+        <v>195</v>
+      </c>
+      <c r="F13" t="s">
+        <v>196</v>
+      </c>
+      <c r="G13" t="s">
+        <v>202</v>
+      </c>
+      <c r="H13" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>20</v>
       </c>
@@ -1093,7 +1233,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>21</v>
       </c>
@@ -1101,21 +1241,27 @@
         <v>46</v>
       </c>
       <c r="C16" t="s">
+        <v>166</v>
+      </c>
+      <c r="D16" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>178</v>
+      </c>
+      <c r="B17" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>184</v>
-      </c>
-      <c r="B17" t="s">
-        <v>48</v>
-      </c>
       <c r="C17" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+      <c r="D17" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1123,7 +1269,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1131,7 +1277,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -1139,7 +1285,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>28</v>
       </c>
@@ -1147,7 +1293,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>29</v>
       </c>
@@ -1155,7 +1301,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -1163,7 +1309,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -1171,7 +1317,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -1179,7 +1325,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>38</v>
       </c>
@@ -1187,7 +1333,7 @@
         <v>42156</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>39</v>
       </c>
@@ -1195,7 +1341,7 @@
         <v>42196</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -1203,7 +1349,7 @@
         <v>5.07</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>41</v>
       </c>
@@ -1211,7 +1357,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -1219,7 +1365,7 @@
         <v>117.82</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>43</v>
       </c>
@@ -1242,7 +1388,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1253,60 +1399,60 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1317,7 +1463,7 @@
         <v>100</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1328,7 +1474,7 @@
         <v>200</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1339,7 +1485,7 @@
         <v>300</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1350,7 +1496,7 @@
         <v>400</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1361,7 +1507,7 @@
         <v>500</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1372,7 +1518,7 @@
         <v>600</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1383,7 +1529,7 @@
         <v>700</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1394,7 +1540,7 @@
         <v>800</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1407,81 +1553,81 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="3" t="s">
-        <v>173</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>174</v>
+        <v>210</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1492,7 +1638,7 @@
         <v>100</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1503,7 +1649,7 @@
         <v>200</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1514,7 +1660,7 @@
         <v>300</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1525,7 +1671,7 @@
         <v>400</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1536,7 +1682,7 @@
         <v>500</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1547,7 +1693,7 @@
         <v>600</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1558,7 +1704,7 @@
         <v>700</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1569,7 +1715,7 @@
         <v>800</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1579,14 +1725,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62AE1033-5819-974F-8B61-434FB3A99D80}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
@@ -1597,42 +1744,42 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -1643,13 +1790,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>64</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
@@ -1660,13 +1807,13 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D4" s="3">
         <v>2480962</v>
@@ -1679,94 +1826,160 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>78</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8">
         <v>5361886</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H8" s="3">
         <v>2480962</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>187</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1793,113 +2006,113 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>84</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>98</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="G6" s="3"/>
     </row>
@@ -1928,30 +2141,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -1960,10 +2173,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1972,10 +2185,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C4" s="3">
         <v>4.9577210000000003</v>
@@ -1984,70 +2197,70 @@
         <v>117.776023</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2060,7 +2273,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2070,73 +2283,73 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>131</v>
       </c>
       <c r="D6" s="3"/>
     </row>
@@ -2216,62 +2429,62 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="3"/>
       <c r="C5" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2279,7 +2492,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C7" s="3">
         <v>24</v>
@@ -2290,7 +2503,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="3">
         <v>12</v>
@@ -2301,7 +2514,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C9" s="3">
         <v>62</v>
@@ -2312,7 +2525,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C10" s="3">
         <v>3</v>
@@ -2328,7 +2541,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2340,78 +2553,78 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -2419,13 +2632,13 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2433,13 +2646,13 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2463,50 +2676,50 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -2514,7 +2727,7 @@
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -2522,7 +2735,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2535,7 +2748,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2547,73 +2760,73 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="3" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2621,10 +2834,10 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2632,10 +2845,10 @@
         <v>2</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>